<commit_message>
Add function to create excel with multiple sheets.
</commit_message>
<xml_diff>
--- a/Estimation.WebApi/Forms/DescriptionOfEstimation_DetailForm.xlsx
+++ b/Estimation.WebApi/Forms/DescriptionOfEstimation_DetailForm.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mattanapol.K\source\repos\EstimationServer\Estimation.WebApi\Forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mattanapol.K\Source\Repos\EstimationServer\Estimation.WebApi\Forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{30B8AE48-5704-4895-B485-BD0A9D1EC919}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Description" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Summary!$1:$5</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Description!$1:$5</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>Date: ##Date##</t>
   </si>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -205,7 +205,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -232,15 +232,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -523,7 +514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -537,7 +528,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -549,93 +540,78 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -648,16 +624,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -973,7 +940,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
@@ -992,18 +959,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
     </row>
     <row r="2" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1034,38 +1001,38 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40" t="s">
+      <c r="F4" s="33"/>
+      <c r="G4" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40" t="s">
+      <c r="H4" s="33"/>
+      <c r="I4" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="42" t="s">
+      <c r="J4" s="35" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="4" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="5" t="s">
         <v>33</v>
       </c>
@@ -1078,8 +1045,8 @@
       <c r="H5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="41"/>
-      <c r="J5" s="43"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="36"/>
     </row>
     <row r="6" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -1096,202 +1063,202 @@
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="20" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="25" t="s">
+      <c r="J8" s="18" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="25"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="18"/>
     </row>
     <row r="10" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="23">
+      <c r="B10" s="15"/>
+      <c r="C10" s="16">
         <v>1</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="23" t="s">
+      <c r="E10" s="17"/>
+      <c r="F10" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="23" t="s">
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="J10" s="25"/>
+      <c r="J10" s="18"/>
     </row>
     <row r="11" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="23">
+      <c r="B11" s="15"/>
+      <c r="C11" s="16">
         <v>1</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="23" t="s">
+      <c r="E11" s="17"/>
+      <c r="F11" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="23" t="s">
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="25"/>
+      <c r="J11" s="18"/>
     </row>
     <row r="12" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="23">
+      <c r="B12" s="15"/>
+      <c r="C12" s="16">
         <v>1</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="23" t="s">
+      <c r="E12" s="17"/>
+      <c r="F12" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="23" t="s">
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="25"/>
+      <c r="J12" s="18"/>
     </row>
     <row r="13" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="23">
+      <c r="B13" s="15"/>
+      <c r="C13" s="16">
         <v>1</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="24"/>
-      <c r="F13" s="23" t="s">
+      <c r="E13" s="17"/>
+      <c r="F13" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="23" t="s">
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="25"/>
+      <c r="J13" s="18"/>
     </row>
     <row r="14" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="44" t="s">
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="23" t="s">
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23" t="s">
+      <c r="G14" s="16"/>
+      <c r="H14" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="23" t="s">
+      <c r="I14" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="J14" s="25"/>
+      <c r="J14" s="18"/>
     </row>
     <row r="15" spans="1:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="31"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="24"/>
     </row>
     <row r="16" spans="1:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="32"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="36" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="34" t="s">
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="34" t="s">
+      <c r="I16" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="J16" s="35"/>
+      <c r="J16" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1310,221 +1277,4 @@
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="60" fitToWidth="0" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:10" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="8"/>
-    </row>
-    <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="13"/>
-    </row>
-    <row r="5" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="12">
-        <v>1</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="13"/>
-    </row>
-    <row r="6" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="12">
-        <v>1</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="13"/>
-    </row>
-    <row r="7" spans="1:10" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="12">
-        <v>1</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="13"/>
-    </row>
-    <row r="8" spans="1:10" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="12">
-        <v>1</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="13"/>
-    </row>
-    <row r="9" spans="1:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="J9" s="13"/>
-    </row>
-    <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C9:E9"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>